<commit_message>
renamed DiffractionLossLib DiffractionLossExcell started blank DiffractionLossLib project added helper to resize array results for excel
</commit_message>
<xml_diff>
--- a/Example/Diffraction of Loss Example.xlsx
+++ b/Example/Diffraction of Loss Example.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FB8611-8038-4BE1-B216-7D58F8F60541}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CD15B0-0AB0-4985-ADEC-4547277A5DE6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2490" yWindow="9090" windowWidth="28800" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="180" windowWidth="28800" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -361,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -373,7 +373,7 @@
     <col min="3" max="3" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -381,7 +381,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -392,7 +392,7 @@
         <v>151.20694599999999</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -403,7 +403,7 @@
         <v>151.22117700000001</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -412,7 +412,7 @@
         <v>162.16239680626285</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -421,68 +421,251 @@
         <v>4298.2118411556376</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9">
-        <f>_xll.MakeList()</f>
+        <f t="array" ref="B9:M10">_xll.MakeList()</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>7</v>
+      </c>
+      <c r="J9">
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <v>9</v>
+      </c>
+      <c r="L9">
+        <v>10</v>
+      </c>
+      <c r="M9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>16</v>
+      </c>
+      <c r="G10">
+        <v>25</v>
+      </c>
+      <c r="H10">
+        <v>36</v>
+      </c>
+      <c r="I10">
+        <v>49</v>
+      </c>
+      <c r="J10">
+        <v>64</v>
+      </c>
+      <c r="K10">
+        <v>81</v>
+      </c>
+      <c r="L10">
+        <v>100</v>
+      </c>
+      <c r="M10">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="str">
+        <f>_xll.FooA()</f>
+        <v>potato</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <f t="array" ref="F14:Q15">_xll.MakeList()</f>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+      <c r="K14">
+        <v>5</v>
+      </c>
+      <c r="L14">
+        <v>6</v>
+      </c>
+      <c r="M14">
+        <v>7</v>
+      </c>
+      <c r="N14">
+        <v>8</v>
+      </c>
+      <c r="O14">
+        <v>9</v>
+      </c>
+      <c r="P14">
+        <v>10</v>
+      </c>
+      <c r="Q14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15">
+        <v>9</v>
+      </c>
+      <c r="J15">
+        <v>16</v>
+      </c>
+      <c r="K15">
+        <v>25</v>
+      </c>
+      <c r="L15">
+        <v>36</v>
+      </c>
+      <c r="M15">
+        <v>49</v>
+      </c>
+      <c r="N15">
+        <v>64</v>
+      </c>
+      <c r="O15">
+        <v>81</v>
+      </c>
+      <c r="P15">
+        <v>100</v>
+      </c>
+      <c r="Q15">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>12</v>
+      </c>
+      <c r="H20">
+        <f t="array" ref="H20:S20">_xll.MakeArrayAndResize(1,12)</f>
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>2</v>
+      </c>
+      <c r="K20">
+        <v>3</v>
+      </c>
+      <c r="L20">
+        <v>4</v>
+      </c>
+      <c r="M20">
+        <v>5</v>
+      </c>
+      <c r="N20">
+        <v>6</v>
+      </c>
+      <c r="O20">
+        <v>7</v>
+      </c>
+      <c r="P20">
+        <v>8</v>
+      </c>
+      <c r="Q20">
+        <v>9</v>
+      </c>
+      <c r="R20">
+        <v>10</v>
+      </c>
+      <c r="S20">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed some scopes/accessibility stuff
</commit_message>
<xml_diff>
--- a/Example/Diffraction of Loss Example.xlsx
+++ b/Example/Diffraction of Loss Example.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CD15B0-0AB0-4985-ADEC-4547277A5DE6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCF93BE-DF78-4F77-93D5-A3C0383B28B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="180" windowWidth="28800" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -361,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -373,7 +373,7 @@
     <col min="3" max="3" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -381,7 +381,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -392,7 +392,7 @@
         <v>151.20694599999999</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -403,7 +403,7 @@
         <v>151.22117700000001</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -412,7 +412,7 @@
         <v>162.16239680626285</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -421,251 +421,101 @@
         <v>4298.2118411556376</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
+        <f t="array" ref="A9:B20">_xll.MakeList()</f>
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>1</v>
       </c>
-      <c r="B9">
-        <f t="array" ref="B9:M10">_xll.MakeList()</f>
-        <v>0</v>
-      </c>
-      <c r="C9">
+      <c r="B10">
         <v>1</v>
       </c>
-      <c r="D9">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>2</v>
       </c>
-      <c r="E9">
+      <c r="B11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>3</v>
       </c>
-      <c r="F9">
+      <c r="B12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>4</v>
       </c>
-      <c r="G9">
+      <c r="B13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>5</v>
       </c>
-      <c r="H9">
+      <c r="B14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>6</v>
       </c>
-      <c r="I9">
+      <c r="B15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>7</v>
       </c>
-      <c r="J9">
+      <c r="B16">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>8</v>
       </c>
-      <c r="K9">
+      <c r="B17">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>9</v>
       </c>
-      <c r="L9">
+      <c r="B18">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>10</v>
       </c>
-      <c r="M9">
+      <c r="B19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>4</v>
-      </c>
-      <c r="E10">
-        <v>9</v>
-      </c>
-      <c r="F10">
-        <v>16</v>
-      </c>
-      <c r="G10">
-        <v>25</v>
-      </c>
-      <c r="H10">
-        <v>36</v>
-      </c>
-      <c r="I10">
-        <v>49</v>
-      </c>
-      <c r="J10">
-        <v>64</v>
-      </c>
-      <c r="K10">
-        <v>81</v>
-      </c>
-      <c r="L10">
-        <v>100</v>
-      </c>
-      <c r="M10">
+      <c r="B20">
         <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>3</v>
-      </c>
-      <c r="D11" t="str">
-        <f>_xll.FooA()</f>
-        <v>potato</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>6</v>
-      </c>
-      <c r="F14">
-        <f t="array" ref="F14:Q15">_xll.MakeList()</f>
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>2</v>
-      </c>
-      <c r="I14">
-        <v>3</v>
-      </c>
-      <c r="J14">
-        <v>4</v>
-      </c>
-      <c r="K14">
-        <v>5</v>
-      </c>
-      <c r="L14">
-        <v>6</v>
-      </c>
-      <c r="M14">
-        <v>7</v>
-      </c>
-      <c r="N14">
-        <v>8</v>
-      </c>
-      <c r="O14">
-        <v>9</v>
-      </c>
-      <c r="P14">
-        <v>10</v>
-      </c>
-      <c r="Q14">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>7</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <v>4</v>
-      </c>
-      <c r="I15">
-        <v>9</v>
-      </c>
-      <c r="J15">
-        <v>16</v>
-      </c>
-      <c r="K15">
-        <v>25</v>
-      </c>
-      <c r="L15">
-        <v>36</v>
-      </c>
-      <c r="M15">
-        <v>49</v>
-      </c>
-      <c r="N15">
-        <v>64</v>
-      </c>
-      <c r="O15">
-        <v>81</v>
-      </c>
-      <c r="P15">
-        <v>100</v>
-      </c>
-      <c r="Q15">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>12</v>
-      </c>
-      <c r="H20">
-        <f t="array" ref="H20:S20">_xll.MakeArrayAndResize(1,12)</f>
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-      <c r="J20">
-        <v>2</v>
-      </c>
-      <c r="K20">
-        <v>3</v>
-      </c>
-      <c r="L20">
-        <v>4</v>
-      </c>
-      <c r="M20">
-        <v>5</v>
-      </c>
-      <c r="N20">
-        <v>6</v>
-      </c>
-      <c r="O20">
-        <v>7</v>
-      </c>
-      <c r="P20">
-        <v>8</v>
-      </c>
-      <c r="Q20">
-        <v>9</v>
-      </c>
-      <c r="R20">
-        <v>10</v>
-      </c>
-      <c r="S20">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed case 1 bullington method added NextPoint Excel function
</commit_message>
<xml_diff>
--- a/Example/Diffraction of Loss Example.xlsx
+++ b/Example/Diffraction of Loss Example.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCF93BE-DF78-4F77-93D5-A3C0383B28B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4069111-1935-4FB7-950E-5643499975B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="180" windowWidth="28800" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="30" windowWidth="28800" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ProfilePoints" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Rx</t>
   </si>
@@ -44,6 +44,12 @@
   </si>
   <si>
     <t>Lon</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>Intermediate Points</t>
   </si>
 </sst>
 </file>
@@ -361,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -373,7 +379,7 @@
     <col min="3" max="3" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -381,7 +387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -392,7 +398,7 @@
         <v>151.20694599999999</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -403,7 +409,7 @@
         <v>151.22117700000001</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -412,110 +418,206 @@
         <v>162.16239680626285</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6">
-        <f>_xll.GetDistance(B2,C2,B3,C3)</f>
-        <v>4298.2118411556376</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="array" ref="A9:B20">_xll.MakeList()</f>
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <f t="array" ref="B8:C8">_xll.NextPoint(B2,C2,B5,B6)</f>
+        <v>-33.848125689319261</v>
+      </c>
+      <c r="C8">
+        <v>151.21025912980389</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
+        <f t="array" ref="A11:C22">_xll.GetProfilePoints(B2,C2,B8,C8)</f>
+        <v>-33.839535000000012</v>
+      </c>
+      <c r="B11">
+        <v>151.20694600000002</v>
+      </c>
+      <c r="C11">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>-33.84039321526285</v>
+      </c>
+      <c r="B12">
+        <v>151.20727695218665</v>
+      </c>
+      <c r="C12">
+        <v>85</v>
+      </c>
+      <c r="D12">
+        <f>_xll.GetDistance(A11,B11,A12,B12)</f>
+        <v>99.999999998559602</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>-33.841251429517683</v>
+      </c>
+      <c r="B13">
+        <v>151.20760791098985</v>
+      </c>
+      <c r="C13">
+        <v>62</v>
+      </c>
+      <c r="D13">
+        <f>_xll.GetDistance(A12,B12,A13,B13)</f>
+        <v>100.00000000021625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-33.842109642764484</v>
+      </c>
+      <c r="B14">
+        <v>151.20793887640997</v>
+      </c>
+      <c r="C14">
+        <v>45</v>
+      </c>
+      <c r="D14">
+        <f>_xll.GetDistance(A13,B13,A14,B14)</f>
+        <v>100.0000000012439</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>-33.842967855003167</v>
+      </c>
+      <c r="B15">
+        <v>151.20826984844734</v>
+      </c>
+      <c r="C15">
+        <v>28</v>
+      </c>
+      <c r="D15">
+        <f>_xll.GetDistance(A14,B14,A15,B15)</f>
+        <v>100.00000000053575</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>-33.843826066233703</v>
+      </c>
+      <c r="B16">
+        <v>151.20860082710232</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <f>_xll.GetDistance(A15,B15,A16,B16)</f>
+        <v>99.999999999583224</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>-33.844684276456036</v>
+      </c>
+      <c r="B17">
+        <v>151.20893181237523</v>
+      </c>
+      <c r="C17">
         <v>2</v>
       </c>
-      <c r="B11">
+      <c r="D17">
+        <f>_xll.GetDistance(A16,B16,A17,B17)</f>
+        <v>99.999999999920746</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>-33.845542485670137</v>
+      </c>
+      <c r="B18">
+        <v>151.20926280426636</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <f>_xll.GetDistance(A17,B17,A18,B18)</f>
+        <v>99.999999998906816</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>-33.84640069387595</v>
+      </c>
+      <c r="B19">
+        <v>151.20959380277611</v>
+      </c>
+      <c r="C19">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>3</v>
-      </c>
-      <c r="B12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>4</v>
-      </c>
-      <c r="B13">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>5</v>
-      </c>
-      <c r="B14">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>6</v>
-      </c>
-      <c r="B15">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="D19">
+        <f>_xll.GetDistance(A18,B18,A19,B19)</f>
+        <v>99.999999999952749</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>-33.847258901073417</v>
+      </c>
+      <c r="B20">
+        <v>151.20992480790483</v>
+      </c>
+      <c r="C20">
+        <v>12</v>
+      </c>
+      <c r="D20">
+        <f>_xll.GetDistance(A19,B19,A20,B20)</f>
+        <v>99.999999998637975</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>-33.848117107262482</v>
+      </c>
+      <c r="B21">
+        <v>151.21025581965284</v>
+      </c>
+      <c r="C21">
         <v>7</v>
       </c>
-      <c r="B16">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>8</v>
-      </c>
-      <c r="B17">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>9</v>
-      </c>
-      <c r="B18">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>10</v>
-      </c>
-      <c r="B19">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>11</v>
-      </c>
-      <c r="B20">
-        <v>121</v>
+      <c r="D21">
+        <f>_xll.GetDistance(A20,B20,A21,B21)</f>
+        <v>99.999999998807837</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>-33.848125689319261</v>
+      </c>
+      <c r="B22">
+        <v>151.21025912980389</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <f>_xll.GetDistance(A21,B21,A22,B22)</f>
+        <v>1.0000000016011392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DiffractionLossLib:   - Spherical Earth component for Loss and Beta = 1.0
UnitTests
  - All test cases and measured against a tolerance

License
  - MIT
</commit_message>
<xml_diff>
--- a/Example/Diffraction of Loss Example.xlsx
+++ b/Example/Diffraction of Loss Example.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3CF70F-9728-48F4-92E7-4659082EEFCA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3441704F-8746-40D2-BFB8-FBAB9007CFD1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28710" yWindow="16260" windowWidth="28800" windowHeight="16050" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="16080" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProfilePoints" sheetId="1" r:id="rId1"/>
@@ -7430,8 +7430,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Y12"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="Y13" sqref="Y13"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7452,7 +7452,7 @@
     <col min="14" max="14" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17" customWidth="1"/>
     <col min="18" max="18" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -7549,7 +7549,7 @@
         <v>149.04732100000001</v>
       </c>
       <c r="E2" s="3">
-        <f>_xll.GetHeight(C2,D2)</f>
+        <f>_xll.GetHeight(C2,D2, "C:\Temp\SRTM-cache\")</f>
         <v>675</v>
       </c>
       <c r="F2" s="2">
@@ -7582,7 +7582,7 @@
         <v>148.971474</v>
       </c>
       <c r="Q2" s="4">
-        <f>_xll.GetHeight(O2,P2)</f>
+        <f>_xll.GetHeight(O2,P2, "C:\Temp\SRTM-cache\")</f>
         <v>676</v>
       </c>
       <c r="R2" s="2">
@@ -7608,7 +7608,7 @@
       </c>
       <c r="Y2" s="6">
         <f>_xll.CalculateDiffractionLoss(C2,D2,L2,O2,P2,M2,F2)</f>
-        <v>-16.996360033546829</v>
+        <v>4.9126283500825183</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -7623,7 +7623,7 @@
         <v>149.04732100000001</v>
       </c>
       <c r="E3" s="3">
-        <f>_xll.GetHeight(C3,D3)</f>
+        <f>_xll.GetHeight(C3,D3, "C:\Temp\SRTM-cache\")</f>
         <v>675</v>
       </c>
       <c r="F3" s="2">
@@ -7656,7 +7656,7 @@
         <v>148.971474</v>
       </c>
       <c r="Q3" s="4">
-        <f>_xll.GetHeight(O3,P3)</f>
+        <f>_xll.GetHeight(O3,P3, "C:\Temp\SRTM-cache\")</f>
         <v>676</v>
       </c>
       <c r="R3" s="2">
@@ -7682,7 +7682,7 @@
       </c>
       <c r="Y3" s="6">
         <f>_xll.CalculateDiffractionLoss(C3,D3,L3,O3,P3,M3,F3)</f>
-        <v>-17.600340648115402</v>
+        <v>4.7888851544973488</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -7697,7 +7697,7 @@
         <v>149.04732100000001</v>
       </c>
       <c r="E4" s="3">
-        <f>_xll.GetHeight(C4,D4)</f>
+        <f>_xll.GetHeight(C4,D4, "C:\Temp\SRTM-cache\")</f>
         <v>675</v>
       </c>
       <c r="F4" s="2">
@@ -7730,7 +7730,7 @@
         <v>148.971474</v>
       </c>
       <c r="Q4" s="4">
-        <f>_xll.GetHeight(O4,P4)</f>
+        <f>_xll.GetHeight(O4,P4, "C:\Temp\SRTM-cache\")</f>
         <v>676</v>
       </c>
       <c r="R4" s="2">
@@ -7756,7 +7756,7 @@
       </c>
       <c r="Y4" s="6">
         <f>_xll.CalculateDiffractionLoss(C4,D4,L4,O4,P4,M4,F4)</f>
-        <v>-17.724162736091849</v>
+        <v>4.7636871133617351</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -7771,7 +7771,7 @@
         <v>149.04732100000001</v>
       </c>
       <c r="E5" s="3">
-        <f>_xll.GetHeight(C5,D5)</f>
+        <f>_xll.GetHeight(C5,D5, "C:\Temp\SRTM-cache\")</f>
         <v>675</v>
       </c>
       <c r="F5" s="2">
@@ -7804,7 +7804,7 @@
         <v>148.971474</v>
       </c>
       <c r="Q5" s="4">
-        <f>_xll.GetHeight(O5,P5)</f>
+        <f>_xll.GetHeight(O5,P5, "C:\Temp\SRTM-cache\")</f>
         <v>676</v>
       </c>
       <c r="R5" s="2">
@@ -7830,7 +7830,7 @@
       </c>
       <c r="Y5" s="6">
         <f>_xll.CalculateDiffractionLoss(C5,D5,L5,O5,P5,M5,F5)</f>
-        <v>-17.600340648115402</v>
+        <v>4.7888851544973488</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -7845,7 +7845,7 @@
         <v>149.04732100000001</v>
       </c>
       <c r="E6" s="3">
-        <f>_xll.GetHeight(C6,D6)</f>
+        <f>_xll.GetHeight(C6,D6, "C:\Temp\SRTM-cache\")</f>
         <v>675</v>
       </c>
       <c r="F6" s="2">
@@ -7878,7 +7878,7 @@
         <v>148.971474</v>
       </c>
       <c r="Q6" s="4">
-        <f>_xll.GetHeight(O6,P6)</f>
+        <f>_xll.GetHeight(O6,P6, "C:\Temp\SRTM-cache\")</f>
         <v>676</v>
       </c>
       <c r="R6" s="2">
@@ -7904,7 +7904,7 @@
       </c>
       <c r="Y6" s="6">
         <f>_xll.CalculateDiffractionLoss(C6,D6,L6,O6,P6,M6,F6)</f>
-        <v>-17.724162736091849</v>
+        <v>4.7636871133617351</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -7919,7 +7919,7 @@
         <v>149.04732100000001</v>
       </c>
       <c r="E7" s="3">
-        <f>_xll.GetHeight(C7,D7)</f>
+        <f>_xll.GetHeight(C7,D7, "C:\Temp\SRTM-cache\")</f>
         <v>675</v>
       </c>
       <c r="F7" s="2">
@@ -7952,7 +7952,7 @@
         <v>148.971474</v>
       </c>
       <c r="Q7" s="4">
-        <f>_xll.GetHeight(O7,P7)</f>
+        <f>_xll.GetHeight(O7,P7, "C:\Temp\SRTM-cache\")</f>
         <v>676</v>
       </c>
       <c r="R7" s="2">
@@ -7978,7 +7978,7 @@
       </c>
       <c r="Y7" s="6">
         <f>_xll.CalculateDiffractionLoss(C7,D7,L7,O7,P7,M7,F7)</f>
-        <v>-16.996360033546829</v>
+        <v>4.9126283500825183</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -7993,7 +7993,7 @@
         <v>149.04732100000001</v>
       </c>
       <c r="E8" s="3">
-        <f>_xll.GetHeight(C8,D8)</f>
+        <f>_xll.GetHeight(C8,D8, "C:\Temp\SRTM-cache\")</f>
         <v>675</v>
       </c>
       <c r="F8" s="2">
@@ -8026,7 +8026,7 @@
         <v>148.90862200000001</v>
       </c>
       <c r="Q8" s="4">
-        <f>_xll.GetHeight(O8,P8)</f>
+        <f>_xll.GetHeight(O8,P8, "C:\Temp\SRTM-cache\")</f>
         <v>539</v>
       </c>
       <c r="R8" s="2">
@@ -8052,7 +8052,7 @@
       </c>
       <c r="Y8" s="6">
         <f>_xll.CalculateDiffractionLoss(C8,D8,L8,O8,P8,M8,F8)</f>
-        <v>41.645241270561741</v>
+        <v>27.583217175888194</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -8067,7 +8067,7 @@
         <v>149.04732100000001</v>
       </c>
       <c r="E9" s="3">
-        <f>_xll.GetHeight(C9,D9)</f>
+        <f>_xll.GetHeight(C9,D9, "C:\Temp\SRTM-cache\")</f>
         <v>675</v>
       </c>
       <c r="F9" s="2">
@@ -8100,7 +8100,7 @@
         <v>148.90862200000001</v>
       </c>
       <c r="Q9" s="4">
-        <f>_xll.GetHeight(O9,P9)</f>
+        <f>_xll.GetHeight(O9,P9, "C:\Temp\SRTM-cache\")</f>
         <v>539</v>
       </c>
       <c r="R9" s="2">
@@ -8126,7 +8126,7 @@
       </c>
       <c r="Y9" s="6">
         <f>_xll.CalculateDiffractionLoss(C9,D9,L9,O9,P9,M9,F9)</f>
-        <v>41.898511850054284</v>
+        <v>27.703098903791002</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="30" x14ac:dyDescent="0.25">
@@ -8141,7 +8141,7 @@
         <v>149.04732100000001</v>
       </c>
       <c r="E10" s="3">
-        <f>_xll.GetHeight(C10,D10)</f>
+        <f>_xll.GetHeight(C10,D10, "C:\Temp\SRTM-cache\")</f>
         <v>675</v>
       </c>
       <c r="F10" s="2">
@@ -8174,7 +8174,7 @@
         <v>148.90862200000001</v>
       </c>
       <c r="Q10" s="4">
-        <f>_xll.GetHeight(O10,P10)</f>
+        <f>_xll.GetHeight(O10,P10, "C:\Temp\SRTM-cache\")</f>
         <v>539</v>
       </c>
       <c r="R10" s="2">
@@ -8200,7 +8200,7 @@
       </c>
       <c r="Y10" s="6">
         <f>_xll.CalculateDiffractionLoss(C10,D10,L10,O10,P10,M10,F10)</f>
-        <v>41.949691938980983</v>
+        <v>27.727306275456513</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
@@ -8213,7 +8213,7 @@
         <v>149.04723055555556</v>
       </c>
       <c r="E11" s="3">
-        <f>_xll.GetHeight(C11,D11)</f>
+        <f>_xll.GetHeight(C11,D11, "C:\Temp\SRTM-cache\")</f>
         <v>675</v>
       </c>
       <c r="F11" s="7">
@@ -8234,12 +8234,12 @@
         <v>148.971475</v>
       </c>
       <c r="Q11" s="4">
-        <f>_xll.GetHeight(O11,P11)</f>
+        <f>_xll.GetHeight(O11,P11, "C:\Temp\SRTM-cache\")</f>
         <v>676</v>
       </c>
       <c r="Y11" s="6">
         <f>_xll.CalculateDiffractionLoss(C11,D11,L11,O11,P11,M11,F11)</f>
-        <v>-17.157228417989494</v>
+        <v>4.8798797952523731</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -8250,7 +8250,7 @@
         <v>150.89236099999999</v>
       </c>
       <c r="E12" s="3">
-        <f>_xll.GetHeight(C12,D12)</f>
+        <f>_xll.GetHeight(C12,D12, "C:\Temp\SRTM-cache\")</f>
         <v>477</v>
       </c>
       <c r="F12" s="9">
@@ -8269,12 +8269,12 @@
         <v>150.39263600000001</v>
       </c>
       <c r="Q12" s="4">
-        <f>_xll.GetHeight(O12,P12)</f>
+        <f>_xll.GetHeight(O12,P12, "C:\Temp\SRTM-cache\")</f>
         <v>322</v>
       </c>
       <c r="Y12" s="6">
         <f>_xll.CalculateDiffractionLoss(C12,D12,L12,O12,P12,M12,F12)</f>
-        <v>83.074918473534225</v>
+        <v>46.305509813189801</v>
       </c>
     </row>
   </sheetData>
@@ -8289,7 +8289,7 @@
   <dimension ref="A1:F461"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14734,7 +14734,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C622"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AE27" sqref="AE27"/>
     </sheetView>
   </sheetViews>
@@ -21576,7 +21576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F9D5F6-4FC2-4FEA-94F4-B964AA6A10E7}">
   <dimension ref="A1:I823"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -21700,12 +21700,12 @@
         <v>-0.32657391255272616</v>
       </c>
       <c r="H9" s="16">
-        <f>6.9 + 20 * LN( SQRT( POWER(G9 - 0.1, 2) + 1) + G9 - 0.1)</f>
-        <v>-1.3918820919201575</v>
+        <f>6.9 + 20 *LOG10( SQRT( POWER(G9 - 0.1, 2) + 1) + G9 - 0.1)</f>
+        <v>3.2988813628866835</v>
       </c>
       <c r="I9" s="16">
         <f>H9 + ((1 - EXP(-H9/6)) * (10 + (0.02 * $A$823)))</f>
-        <v>-4.2143765663423753</v>
+        <v>7.8709851349471016</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -44438,8 +44438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988C331D-5211-4E01-AF92-9A5881DA4A1C}">
   <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45087,8 +45087,8 @@
         <v>66</v>
       </c>
       <c r="C47">
-        <f>6.9 + 20 * LN( SQRT( POWER(G43 - 0.1, 2) + 1) + G43 - 0.1)</f>
-        <v>-7.6277318824237135</v>
+        <f>6.9 + 20 *LOG10( SQRT( POWER(G43 - 0.1, 2) + 1) + G43 - 0.1)</f>
+        <v>0.59068620889344015</v>
       </c>
       <c r="E47" t="s">
         <v>79</v>
@@ -45153,8 +45153,8 @@
         <v>73</v>
       </c>
       <c r="F54">
-        <f>LN(F53)</f>
-        <v>-0.72638659412118567</v>
+        <f>LOG10(F53)</f>
+        <v>-0.315465689555328</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -45163,7 +45163,7 @@
       </c>
       <c r="F55">
         <f>20 *F54</f>
-        <v>-14.527731882423714</v>
+        <v>-6.3093137911065602</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -45172,7 +45172,7 @@
       </c>
       <c r="F56">
         <f>6.9 + F55</f>
-        <v>-7.6277318824237135</v>
+        <v>0.59068620889344015</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -45186,7 +45186,7 @@
       </c>
       <c r="C60">
         <f>C47 + ((1 - EXP(-C47/6)) * (10 + (0.02 * B42)))</f>
-        <v>-33.30782834890087</v>
+        <v>1.5291929125769859</v>
       </c>
       <c r="E60" t="s">
         <v>81</v>
@@ -45206,14 +45206,14 @@
         <v>86</v>
       </c>
       <c r="C62">
-        <v>-33.307828348900799</v>
+        <v>1.5291929125769801</v>
       </c>
       <c r="E62" s="11" t="s">
         <v>82</v>
       </c>
       <c r="F62">
         <f>-C47/6</f>
-        <v>1.2712886470706188</v>
+        <v>-9.8447701482240024E-2</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -45222,7 +45222,7 @@
       </c>
       <c r="F63">
         <f xml:space="preserve"> 1 - EXP(F62)</f>
-        <v>-2.5654442024452702</v>
+        <v>9.3756913454899671E-2</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -45231,7 +45231,7 @@
       </c>
       <c r="F64">
         <f>C47 + (F63 * F61)</f>
-        <v>-33.284739351078855</v>
+        <v>1.5283491003558916</v>
       </c>
     </row>
   </sheetData>

</xml_diff>